<commit_message>
Calibration Legs and Others Update!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lazy_Panda\Documents\GitHub\New 2\Sesi 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lazy_Panda\Documents\GitHub2\tirtapods-x\krpai2020\Sesi 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -509,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -656,10 +656,10 @@
         <v>1600</v>
       </c>
       <c r="D5" s="1">
-        <v>1550</v>
+        <v>1600</v>
       </c>
       <c r="E5" s="1">
-        <v>950</v>
+        <v>1000</v>
       </c>
       <c r="F5" s="1">
         <v>2070</v>
@@ -669,7 +669,7 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H9" si="0">D5-2*(D5-G5)</f>
-        <v>2450</v>
+        <v>2400</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I9" si="1">C5</f>
@@ -681,7 +681,7 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K9" si="2">D5-G5</f>
-        <v>-450</v>
+        <v>-400</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L9" si="3">F5-C5</f>
@@ -689,7 +689,7 @@
       </c>
       <c r="M5" s="1">
         <f>E5-B5</f>
-        <v>-450</v>
+        <v>-400</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -697,7 +697,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>1490</v>
+        <v>1400</v>
       </c>
       <c r="C6" s="1">
         <v>1400</v>
@@ -736,7 +736,7 @@
       </c>
       <c r="M6" s="1">
         <f>B6-E6</f>
-        <v>540</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -791,16 +791,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>1545</v>
+        <v>1400</v>
       </c>
       <c r="C8" s="1">
-        <v>1550</v>
+        <v>1500</v>
       </c>
       <c r="D8" s="1">
-        <v>1280</v>
+        <v>1200</v>
       </c>
       <c r="E8" s="1">
-        <v>2000</v>
+        <v>1850</v>
       </c>
       <c r="F8" s="1">
         <v>1040</v>
@@ -810,27 +810,27 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>400</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1500</v>
       </c>
       <c r="J8" s="1">
         <f>B8</f>
-        <v>1545</v>
+        <v>1400</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>-510</v>
+        <v>-460</v>
       </c>
       <c r="M8" s="1">
         <f>E8-B8</f>
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>1360</v>
+        <v>1300</v>
       </c>
       <c r="C9" s="1">
         <v>1400</v>
@@ -847,7 +847,7 @@
         <v>1400</v>
       </c>
       <c r="E9" s="1">
-        <v>1840</v>
+        <v>1800</v>
       </c>
       <c r="F9" s="1">
         <v>900</v>
@@ -865,7 +865,7 @@
       </c>
       <c r="J9" s="1">
         <f>E9</f>
-        <v>1840</v>
+        <v>1800</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
@@ -877,7 +877,7 @@
       </c>
       <c r="M9" s="1">
         <f>B9-E9</f>
-        <v>-480</v>
+        <v>-500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transpiler and Automatic calculator!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lazy_Panda\Documents\GitHub2\tirtapods-x\krpai2020\Sesi 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lazy_Panda\Documents\GitHub2\tirtapods-x\krpai2020\Sesi 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -510,7 +510,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,10 +700,10 @@
         <v>1400</v>
       </c>
       <c r="C6" s="1">
-        <v>1400</v>
+        <v>1350</v>
       </c>
       <c r="D6" s="1">
-        <v>1600</v>
+        <v>1550</v>
       </c>
       <c r="E6" s="1">
         <v>950</v>
@@ -716,11 +716,11 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2500</v>
+        <v>2550</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>1400</v>
+        <v>1350</v>
       </c>
       <c r="J6" s="1">
         <f>E6</f>
@@ -728,11 +728,11 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-450</v>
+        <v>-500</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="M6" s="1">
         <f>B6-E6</f>
@@ -797,7 +797,7 @@
         <v>1500</v>
       </c>
       <c r="D8" s="1">
-        <v>1200</v>
+        <v>1250</v>
       </c>
       <c r="E8" s="1">
         <v>1850</v>
@@ -810,7 +810,7 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
@@ -822,7 +822,7 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Legs and Room 3 Sesi 2 Update!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F0E0BC-CBA3-4C27-8D8B-41957985DF5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902845EB-1014-4EA8-801F-809A9C2C5D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="2175" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,27 +613,27 @@
         <v>1400</v>
       </c>
       <c r="C4" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D4" s="1">
         <v>1550</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1500</v>
       </c>
       <c r="E4" s="1">
         <v>900</v>
       </c>
       <c r="F4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G4" s="1">
         <v>2100</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2050</v>
       </c>
       <c r="H4" s="1">
         <f>D4-2*(D4-G4)</f>
-        <v>2600</v>
+        <v>2650</v>
       </c>
       <c r="I4" s="1">
         <f>C4</f>
-        <v>1550</v>
+        <v>1500</v>
       </c>
       <c r="J4" s="1">
         <f>E4-2*(E4-B4)</f>
@@ -645,7 +645,7 @@
       </c>
       <c r="L4" s="1">
         <f>F4-C4</f>
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="M4" s="1">
         <f>E4-B4</f>
@@ -663,7 +663,7 @@
         <v>1600</v>
       </c>
       <c r="D5" s="1">
-        <v>1500</v>
+        <v>1450</v>
       </c>
       <c r="E5" s="1">
         <v>1000</v>
@@ -676,7 +676,7 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H9" si="0">D5-2*(D5-G5)</f>
-        <v>2400</v>
+        <v>2450</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I9" si="1">C5</f>
@@ -688,7 +688,7 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K9" si="2">D5-G5</f>
-        <v>-450</v>
+        <v>-500</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L9" si="3">F5-C5</f>
@@ -707,10 +707,10 @@
         <v>1450</v>
       </c>
       <c r="C6" s="1">
-        <v>1250</v>
+        <v>1350</v>
       </c>
       <c r="D6" s="1">
-        <v>1500</v>
+        <v>1650</v>
       </c>
       <c r="E6" s="1">
         <v>950</v>
@@ -723,11 +723,11 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2600</v>
+        <v>2450</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>1250</v>
+        <v>1350</v>
       </c>
       <c r="J6" s="1">
         <f>E6</f>
@@ -735,11 +735,11 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-550</v>
+        <v>-400</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="M6" s="1">
         <f>B6-E6</f>
@@ -757,7 +757,7 @@
         <v>1400</v>
       </c>
       <c r="D7" s="1">
-        <v>1380</v>
+        <v>1350</v>
       </c>
       <c r="E7" s="1">
         <v>2000</v>
@@ -766,11 +766,11 @@
         <v>940</v>
       </c>
       <c r="G7" s="1">
-        <v>900</v>
+        <v>850</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>420</v>
+        <v>350</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
@@ -782,7 +782,7 @@
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>500</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
@@ -801,13 +801,13 @@
         <v>1400</v>
       </c>
       <c r="C8" s="1">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="D8" s="1">
-        <v>1250</v>
+        <v>1300</v>
       </c>
       <c r="E8" s="1">
-        <v>1850</v>
+        <v>1870</v>
       </c>
       <c r="F8" s="1">
         <v>1040</v>
@@ -817,11 +817,11 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="J8" s="1">
         <f>B8</f>
@@ -829,15 +829,15 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>-460</v>
+        <v>-510</v>
       </c>
       <c r="M8" s="1">
         <f>E8-B8</f>
-        <v>450</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Legs and Sesi 2 Update!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902845EB-1014-4EA8-801F-809A9C2C5D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277E2F2C-6B0C-4885-B0FA-418B9C5B72C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="2175" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="2175" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +660,10 @@
         <v>1450</v>
       </c>
       <c r="C5" s="1">
+        <v>1620</v>
+      </c>
+      <c r="D5" s="1">
         <v>1600</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1450</v>
       </c>
       <c r="E5" s="1">
         <v>1000</v>
@@ -672,15 +672,15 @@
         <v>2100</v>
       </c>
       <c r="G5" s="1">
-        <v>1950</v>
+        <v>2070</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H9" si="0">D5-2*(D5-G5)</f>
-        <v>2450</v>
+        <v>2540</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I9" si="1">C5</f>
-        <v>1600</v>
+        <v>1620</v>
       </c>
       <c r="J5" s="1">
         <f>B5</f>
@@ -688,11 +688,11 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K9" si="2">D5-G5</f>
-        <v>-500</v>
+        <v>-470</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L9" si="3">F5-C5</f>
-        <v>500</v>
+        <v>480</v>
       </c>
       <c r="M5" s="1">
         <f>E5-B5</f>
@@ -719,11 +719,11 @@
         <v>1850</v>
       </c>
       <c r="G6" s="1">
-        <v>2050</v>
+        <v>2100</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2450</v>
+        <v>2550</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
@@ -735,7 +735,7 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-400</v>
+        <v>-450</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
@@ -804,7 +804,7 @@
         <v>1550</v>
       </c>
       <c r="D8" s="1">
-        <v>1300</v>
+        <v>1320</v>
       </c>
       <c r="E8" s="1">
         <v>1870</v>
@@ -817,7 +817,7 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
@@ -829,7 +829,7 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>450</v>
+        <v>470</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
@@ -851,7 +851,7 @@
         <v>1400</v>
       </c>
       <c r="D9" s="1">
-        <v>1400</v>
+        <v>1250</v>
       </c>
       <c r="E9" s="1">
         <v>1800</v>
@@ -860,11 +860,11 @@
         <v>900</v>
       </c>
       <c r="G9" s="1">
-        <v>850</v>
+        <v>800</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
@@ -876,7 +876,7 @@
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>550</v>
+        <v>450</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Legs Update and Sesi 1,2,3 Update
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB4CB5C-97ED-4D8A-82D9-CBB0CAF478CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ED7E79-0ACF-4776-A070-8CA45931DFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="2175" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6810" yWindow="1170" windowWidth="15195" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +613,7 @@
         <v>1400</v>
       </c>
       <c r="C4" s="1">
-        <v>1500</v>
+        <v>1430</v>
       </c>
       <c r="D4" s="1">
         <v>1600</v>
@@ -622,7 +622,7 @@
         <v>900</v>
       </c>
       <c r="F4" s="1">
-        <v>2000</v>
+        <v>1950</v>
       </c>
       <c r="G4" s="1">
         <v>2100</v>
@@ -633,7 +633,7 @@
       </c>
       <c r="I4" s="1">
         <f>C4</f>
-        <v>1500</v>
+        <v>1430</v>
       </c>
       <c r="J4" s="1">
         <f>E4-2*(E4-B4)</f>
@@ -645,7 +645,7 @@
       </c>
       <c r="L4" s="1">
         <f>F4-C4</f>
-        <v>500</v>
+        <v>520</v>
       </c>
       <c r="M4" s="1">
         <f>E4-B4</f>
@@ -660,10 +660,10 @@
         <v>1450</v>
       </c>
       <c r="C5" s="1">
-        <v>1600</v>
+        <v>1580</v>
       </c>
       <c r="D5" s="1">
-        <v>1600</v>
+        <v>1570</v>
       </c>
       <c r="E5" s="1">
         <v>1000</v>
@@ -672,15 +672,15 @@
         <v>2100</v>
       </c>
       <c r="G5" s="1">
-        <v>2120</v>
+        <v>2000</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H9" si="0">D5-2*(D5-G5)</f>
-        <v>2640</v>
+        <v>2430</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I9" si="1">C5</f>
-        <v>1600</v>
+        <v>1580</v>
       </c>
       <c r="J5" s="1">
         <f>B5</f>
@@ -688,11 +688,11 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K9" si="2">D5-G5</f>
-        <v>-520</v>
+        <v>-430</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L9" si="3">F5-C5</f>
-        <v>500</v>
+        <v>520</v>
       </c>
       <c r="M5" s="1">
         <f>E5-B5</f>
@@ -707,10 +707,10 @@
         <v>1350</v>
       </c>
       <c r="C6" s="1">
-        <v>1350</v>
+        <v>1400</v>
       </c>
       <c r="D6" s="1">
-        <v>1620</v>
+        <v>1680</v>
       </c>
       <c r="E6" s="1">
         <v>900</v>
@@ -719,15 +719,15 @@
         <v>1850</v>
       </c>
       <c r="G6" s="1">
-        <v>2100</v>
+        <v>2150</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2580</v>
+        <v>2620</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>1350</v>
+        <v>1400</v>
       </c>
       <c r="J6" s="1">
         <f>E6</f>
@@ -735,11 +735,11 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-480</v>
+        <v>-470</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="M6" s="1">
         <f>B6-E6</f>
@@ -804,7 +804,7 @@
         <v>1550</v>
       </c>
       <c r="D8" s="1">
-        <v>1250</v>
+        <v>1200</v>
       </c>
       <c r="E8" s="1">
         <v>1870</v>
@@ -813,11 +813,11 @@
         <v>1040</v>
       </c>
       <c r="G8" s="1">
-        <v>750</v>
+        <v>730</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
@@ -829,7 +829,7 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>500</v>
+        <v>470</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
@@ -848,43 +848,43 @@
         <v>1350</v>
       </c>
       <c r="C9" s="1">
-        <v>1350</v>
+        <v>1430</v>
       </c>
       <c r="D9" s="1">
-        <v>1280</v>
+        <v>1230</v>
       </c>
       <c r="E9" s="1">
-        <v>1850</v>
+        <v>1830</v>
       </c>
       <c r="F9" s="1">
-        <v>850</v>
+        <v>900</v>
       </c>
       <c r="G9" s="1">
         <v>750</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>1350</v>
+        <v>1430</v>
       </c>
       <c r="J9" s="1">
         <f>E9</f>
-        <v>1850</v>
+        <v>1830</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>530</v>
+        <v>480</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>-500</v>
+        <v>-530</v>
       </c>
       <c r="M9" s="1">
         <f>B9-E9</f>
-        <v>-500</v>
+        <v>-480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Legs Update and Sesi 2 Update!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ED7E79-0ACF-4776-A070-8CA45931DFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FD52D6-C40C-4F73-8152-07245806570B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="1170" windowWidth="15195" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5295" yWindow="1170" windowWidth="15195" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +663,7 @@
         <v>1580</v>
       </c>
       <c r="D5" s="1">
-        <v>1570</v>
+        <v>1580</v>
       </c>
       <c r="E5" s="1">
         <v>1000</v>
@@ -672,11 +672,11 @@
         <v>2100</v>
       </c>
       <c r="G5" s="1">
-        <v>2000</v>
+        <v>2050</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H9" si="0">D5-2*(D5-G5)</f>
-        <v>2430</v>
+        <v>2520</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I9" si="1">C5</f>
@@ -688,7 +688,7 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K9" si="2">D5-G5</f>
-        <v>-430</v>
+        <v>-470</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L9" si="3">F5-C5</f>
@@ -804,7 +804,7 @@
         <v>1550</v>
       </c>
       <c r="D8" s="1">
-        <v>1200</v>
+        <v>1250</v>
       </c>
       <c r="E8" s="1">
         <v>1870</v>
@@ -817,7 +817,7 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
@@ -829,7 +829,7 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>470</v>
+        <v>520</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Legs Update and Sesi 1 Update!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FD52D6-C40C-4F73-8152-07245806570B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186322F3-EDB7-44E2-9DAA-AAE76443BEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="1170" windowWidth="15195" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7335" yWindow="720" windowWidth="15195" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,11 +719,11 @@
         <v>1850</v>
       </c>
       <c r="G6" s="1">
-        <v>2150</v>
+        <v>2120</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2620</v>
+        <v>2560</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
@@ -735,7 +735,7 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-470</v>
+        <v>-440</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
@@ -804,7 +804,7 @@
         <v>1550</v>
       </c>
       <c r="D8" s="1">
-        <v>1250</v>
+        <v>1270</v>
       </c>
       <c r="E8" s="1">
         <v>1870</v>
@@ -813,11 +813,11 @@
         <v>1040</v>
       </c>
       <c r="G8" s="1">
-        <v>730</v>
+        <v>750</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
@@ -848,10 +848,10 @@
         <v>1350</v>
       </c>
       <c r="C9" s="1">
-        <v>1430</v>
+        <v>1400</v>
       </c>
       <c r="D9" s="1">
-        <v>1230</v>
+        <v>1250</v>
       </c>
       <c r="E9" s="1">
         <v>1830</v>
@@ -864,11 +864,11 @@
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>1430</v>
+        <v>1400</v>
       </c>
       <c r="J9" s="1">
         <f>E9</f>
@@ -876,11 +876,11 @@
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>500</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>-530</v>
+        <v>-500</v>
       </c>
       <c r="M9" s="1">
         <f>B9-E9</f>

</xml_diff>

<commit_message>
Legs and Sesi 1 Update!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186322F3-EDB7-44E2-9DAA-AAE76443BEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF702B9-394F-4556-9C6B-EAFBC3B7E7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7335" yWindow="720" windowWidth="15195" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5295" yWindow="720" windowWidth="15195" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,20 +616,20 @@
         <v>1430</v>
       </c>
       <c r="D4" s="1">
-        <v>1600</v>
+        <v>1560</v>
       </c>
       <c r="E4" s="1">
         <v>900</v>
       </c>
       <c r="F4" s="1">
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="G4" s="1">
-        <v>2100</v>
+        <v>2120</v>
       </c>
       <c r="H4" s="1">
         <f>D4-2*(D4-G4)</f>
-        <v>2600</v>
+        <v>2680</v>
       </c>
       <c r="I4" s="1">
         <f>C4</f>
@@ -641,11 +641,11 @@
       </c>
       <c r="K4" s="1">
         <f>D4-G4</f>
-        <v>-500</v>
+        <v>-560</v>
       </c>
       <c r="L4" s="1">
         <f>F4-C4</f>
-        <v>520</v>
+        <v>570</v>
       </c>
       <c r="M4" s="1">
         <f>E4-B4</f>
@@ -710,7 +710,7 @@
         <v>1400</v>
       </c>
       <c r="D6" s="1">
-        <v>1680</v>
+        <v>1720</v>
       </c>
       <c r="E6" s="1">
         <v>900</v>
@@ -719,11 +719,11 @@
         <v>1850</v>
       </c>
       <c r="G6" s="1">
-        <v>2120</v>
+        <v>2150</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2560</v>
+        <v>2580</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
@@ -735,7 +735,7 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-440</v>
+        <v>-430</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Legs and Home Update Sesi 2!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF702B9-394F-4556-9C6B-EAFBC3B7E7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F789224-9F6B-43EF-8931-789D4AFD0F12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="720" windowWidth="15195" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5295" yWindow="720" windowWidth="15195" windowHeight="7875" tabRatio="442" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,20 +616,20 @@
         <v>1430</v>
       </c>
       <c r="D4" s="1">
-        <v>1560</v>
+        <v>1580</v>
       </c>
       <c r="E4" s="1">
         <v>900</v>
       </c>
       <c r="F4" s="1">
-        <v>2000</v>
+        <v>1950</v>
       </c>
       <c r="G4" s="1">
-        <v>2120</v>
+        <v>2050</v>
       </c>
       <c r="H4" s="1">
         <f>D4-2*(D4-G4)</f>
-        <v>2680</v>
+        <v>2520</v>
       </c>
       <c r="I4" s="1">
         <f>C4</f>
@@ -641,11 +641,11 @@
       </c>
       <c r="K4" s="1">
         <f>D4-G4</f>
-        <v>-560</v>
+        <v>-470</v>
       </c>
       <c r="L4" s="1">
         <f>F4-C4</f>
-        <v>570</v>
+        <v>520</v>
       </c>
       <c r="M4" s="1">
         <f>E4-B4</f>
@@ -660,10 +660,10 @@
         <v>1450</v>
       </c>
       <c r="C5" s="1">
-        <v>1580</v>
+        <v>1570</v>
       </c>
       <c r="D5" s="1">
-        <v>1580</v>
+        <v>1550</v>
       </c>
       <c r="E5" s="1">
         <v>1000</v>
@@ -676,11 +676,11 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H9" si="0">D5-2*(D5-G5)</f>
-        <v>2520</v>
+        <v>2550</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I9" si="1">C5</f>
-        <v>1580</v>
+        <v>1570</v>
       </c>
       <c r="J5" s="1">
         <f>B5</f>
@@ -688,11 +688,11 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K9" si="2">D5-G5</f>
-        <v>-470</v>
+        <v>-500</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L9" si="3">F5-C5</f>
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="M5" s="1">
         <f>E5-B5</f>
@@ -707,10 +707,10 @@
         <v>1350</v>
       </c>
       <c r="C6" s="1">
-        <v>1400</v>
+        <v>1350</v>
       </c>
       <c r="D6" s="1">
-        <v>1720</v>
+        <v>1680</v>
       </c>
       <c r="E6" s="1">
         <v>900</v>
@@ -723,11 +723,11 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2580</v>
+        <v>2620</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>1400</v>
+        <v>1350</v>
       </c>
       <c r="J6" s="1">
         <f>E6</f>
@@ -735,11 +735,11 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-430</v>
+        <v>-470</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="M6" s="1">
         <f>B6-E6</f>
@@ -754,10 +754,10 @@
         <v>1500</v>
       </c>
       <c r="C7" s="1">
-        <v>1450</v>
+        <v>1410</v>
       </c>
       <c r="D7" s="1">
-        <v>1400</v>
+        <v>1380</v>
       </c>
       <c r="E7" s="1">
         <v>2000</v>
@@ -770,11 +770,11 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>1450</v>
+        <v>1410</v>
       </c>
       <c r="J7" s="1">
         <f>E7-2*(E7-B7)</f>
@@ -782,11 +782,11 @@
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>-510</v>
+        <v>-470</v>
       </c>
       <c r="M7" s="1">
         <f>E7-B7</f>
@@ -801,10 +801,10 @@
         <v>1400</v>
       </c>
       <c r="C8" s="1">
-        <v>1550</v>
+        <v>1600</v>
       </c>
       <c r="D8" s="1">
-        <v>1270</v>
+        <v>1250</v>
       </c>
       <c r="E8" s="1">
         <v>1870</v>
@@ -817,11 +817,11 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1600</v>
       </c>
       <c r="J8" s="1">
         <f>B8</f>
@@ -829,11 +829,11 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>520</v>
+        <v>500</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>-510</v>
+        <v>-560</v>
       </c>
       <c r="M8" s="1">
         <f>E8-B8</f>

</xml_diff>

<commit_message>
Legs Update Sesi 1!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DONNY\Documents\tirtapods-x\krpai2020\Sesi 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471695AA-B74D-48D0-8AD4-2A077E3144FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F52D90E-0ACB-4A82-82D5-AB14D1231064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" tabRatio="442" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5295" yWindow="720" windowWidth="15195" windowHeight="7875" tabRatio="442" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,12 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -510,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="C4" s="1">
         <v>1430</v>
@@ -613,17 +619,17 @@
         <v>1580</v>
       </c>
       <c r="E4" s="1">
-        <v>900</v>
+        <v>950</v>
       </c>
       <c r="F4" s="1">
         <v>1950</v>
       </c>
       <c r="G4" s="1">
-        <v>2050</v>
+        <v>2100</v>
       </c>
       <c r="H4" s="1">
         <f>D4-2*(D4-G4)</f>
-        <v>2520</v>
+        <v>2620</v>
       </c>
       <c r="I4" s="1">
         <f>C4</f>
@@ -631,11 +637,11 @@
       </c>
       <c r="J4" s="1">
         <f>E4-2*(E4-B4)</f>
-        <v>1900</v>
+        <v>2050</v>
       </c>
       <c r="K4" s="1">
         <f>D4-G4</f>
-        <v>-470</v>
+        <v>-520</v>
       </c>
       <c r="L4" s="1">
         <f>F4-C4</f>
@@ -643,7 +649,7 @@
       </c>
       <c r="M4" s="1">
         <f>E4-B4</f>
-        <v>-500</v>
+        <v>-550</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -651,13 +657,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>1450</v>
+        <v>1400</v>
       </c>
       <c r="C5" s="1">
-        <v>1520</v>
+        <v>1550</v>
       </c>
       <c r="D5" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="E5" s="1">
         <v>1000</v>
@@ -666,31 +672,31 @@
         <v>2080</v>
       </c>
       <c r="G5" s="1">
-        <v>2030</v>
+        <v>2150</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H9" si="0">D5-2*(D5-G5)</f>
-        <v>2560</v>
+        <v>2700</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I9" si="1">C5</f>
-        <v>1520</v>
+        <v>1550</v>
       </c>
       <c r="J5" s="1">
         <f>B5</f>
-        <v>1450</v>
+        <v>1400</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K9" si="2">D5-G5</f>
-        <v>-530</v>
+        <v>-550</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L9" si="3">F5-C5</f>
-        <v>560</v>
+        <v>530</v>
       </c>
       <c r="M5" s="1">
         <f>E5-B5</f>
-        <v>-450</v>
+        <v>-400</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -698,19 +704,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>1350</v>
+        <v>1400</v>
       </c>
       <c r="C6" s="1">
-        <v>1350</v>
+        <v>1300</v>
       </c>
       <c r="D6" s="1">
         <v>1680</v>
       </c>
       <c r="E6" s="1">
-        <v>900</v>
+        <v>850</v>
       </c>
       <c r="F6" s="1">
-        <v>1850</v>
+        <v>1800</v>
       </c>
       <c r="G6" s="1">
         <v>2150</v>
@@ -721,11 +727,11 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>1350</v>
+        <v>1300</v>
       </c>
       <c r="J6" s="1">
         <f>E6</f>
-        <v>900</v>
+        <v>850</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
@@ -737,7 +743,7 @@
       </c>
       <c r="M6" s="1">
         <f>B6-E6</f>
-        <v>450</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -745,46 +751,46 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C7" s="1">
         <v>1500</v>
       </c>
-      <c r="C7" s="1">
-        <v>1410</v>
-      </c>
       <c r="D7" s="1">
-        <v>1380</v>
+        <v>1400</v>
       </c>
       <c r="E7" s="1">
-        <v>2000</v>
+        <v>2050</v>
       </c>
       <c r="F7" s="1">
-        <v>940</v>
+        <v>1000</v>
       </c>
       <c r="G7" s="1">
         <v>850</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>1410</v>
+        <v>1500</v>
       </c>
       <c r="J7" s="1">
         <f>E7-2*(E7-B7)</f>
-        <v>1000</v>
+        <v>1150</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>530</v>
+        <v>550</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>-470</v>
+        <v>-500</v>
       </c>
       <c r="M7" s="1">
         <f>E7-B7</f>
-        <v>500</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -792,13 +798,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="C8" s="1">
-        <v>1600</v>
+        <v>1550</v>
       </c>
       <c r="D8" s="1">
-        <v>1250</v>
+        <v>1200</v>
       </c>
       <c r="E8" s="1">
         <v>1870</v>
@@ -807,31 +813,31 @@
         <v>1040</v>
       </c>
       <c r="G8" s="1">
-        <v>750</v>
+        <v>650</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>1600</v>
+        <v>1550</v>
       </c>
       <c r="J8" s="1">
         <f>B8</f>
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>-560</v>
+        <v>-510</v>
       </c>
       <c r="M8" s="1">
         <f>E8-B8</f>
-        <v>470</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -839,34 +845,34 @@
         <v>6</v>
       </c>
       <c r="B9" s="1">
+        <v>1300</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1450</v>
+      </c>
+      <c r="D9" s="1">
         <v>1350</v>
       </c>
-      <c r="C9" s="1">
-        <v>1400</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1250</v>
-      </c>
       <c r="E9" s="1">
-        <v>1830</v>
+        <v>1800</v>
       </c>
       <c r="F9" s="1">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="G9" s="1">
-        <v>750</v>
+        <v>850</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="J9" s="1">
         <f>E9</f>
-        <v>1830</v>
+        <v>1800</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
@@ -874,11 +880,11 @@
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>-500</v>
+        <v>-450</v>
       </c>
       <c r="M9" s="1">
         <f>B9-E9</f>
-        <v>-480</v>
+        <v>-500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Legs Update Sesi 1 and Added Room4Counter!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F52D90E-0ACB-4A82-82D5-AB14D1231064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAB57F4-BB50-48AC-B885-175EC96BACC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5295" yWindow="720" windowWidth="15195" windowHeight="7875" tabRatio="442" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,10 +613,10 @@
         <v>1500</v>
       </c>
       <c r="C4" s="1">
-        <v>1430</v>
+        <v>1480</v>
       </c>
       <c r="D4" s="1">
-        <v>1580</v>
+        <v>1640</v>
       </c>
       <c r="E4" s="1">
         <v>950</v>
@@ -629,11 +629,11 @@
       </c>
       <c r="H4" s="1">
         <f>D4-2*(D4-G4)</f>
-        <v>2620</v>
+        <v>2560</v>
       </c>
       <c r="I4" s="1">
         <f>C4</f>
-        <v>1430</v>
+        <v>1480</v>
       </c>
       <c r="J4" s="1">
         <f>E4-2*(E4-B4)</f>
@@ -641,11 +641,11 @@
       </c>
       <c r="K4" s="1">
         <f>D4-G4</f>
-        <v>-520</v>
+        <v>-460</v>
       </c>
       <c r="L4" s="1">
         <f>F4-C4</f>
-        <v>520</v>
+        <v>470</v>
       </c>
       <c r="M4" s="1">
         <f>E4-B4</f>
@@ -660,27 +660,27 @@
         <v>1400</v>
       </c>
       <c r="C5" s="1">
-        <v>1550</v>
+        <v>1600</v>
       </c>
       <c r="D5" s="1">
-        <v>1600</v>
+        <v>1650</v>
       </c>
       <c r="E5" s="1">
-        <v>1000</v>
+        <v>880</v>
       </c>
       <c r="F5" s="1">
-        <v>2080</v>
+        <v>2100</v>
       </c>
       <c r="G5" s="1">
-        <v>2150</v>
+        <v>2140</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H9" si="0">D5-2*(D5-G5)</f>
-        <v>2700</v>
+        <v>2630</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I9" si="1">C5</f>
-        <v>1550</v>
+        <v>1600</v>
       </c>
       <c r="J5" s="1">
         <f>B5</f>
@@ -688,15 +688,15 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K9" si="2">D5-G5</f>
-        <v>-550</v>
+        <v>-490</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L9" si="3">F5-C5</f>
-        <v>530</v>
+        <v>500</v>
       </c>
       <c r="M5" s="1">
         <f>E5-B5</f>
-        <v>-400</v>
+        <v>-520</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>1400</v>
       </c>
       <c r="C6" s="1">
-        <v>1300</v>
+        <v>1280</v>
       </c>
       <c r="D6" s="1">
         <v>1680</v>
@@ -719,15 +719,15 @@
         <v>1800</v>
       </c>
       <c r="G6" s="1">
-        <v>2150</v>
+        <v>2180</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2620</v>
+        <v>2680</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>1300</v>
+        <v>1280</v>
       </c>
       <c r="J6" s="1">
         <f>E6</f>
@@ -735,11 +735,11 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-470</v>
+        <v>-500</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>520</v>
       </c>
       <c r="M6" s="1">
         <f>B6-E6</f>
@@ -757,7 +757,7 @@
         <v>1500</v>
       </c>
       <c r="D7" s="1">
-        <v>1400</v>
+        <v>1350</v>
       </c>
       <c r="E7" s="1">
         <v>2050</v>
@@ -770,7 +770,7 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
@@ -782,7 +782,7 @@
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
@@ -801,13 +801,13 @@
         <v>1450</v>
       </c>
       <c r="C8" s="1">
-        <v>1550</v>
+        <v>1540</v>
       </c>
       <c r="D8" s="1">
         <v>1200</v>
       </c>
       <c r="E8" s="1">
-        <v>1870</v>
+        <v>1950</v>
       </c>
       <c r="F8" s="1">
         <v>1040</v>
@@ -821,7 +821,7 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1540</v>
       </c>
       <c r="J8" s="1">
         <f>B8</f>
@@ -833,11 +833,11 @@
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>-510</v>
+        <v>-500</v>
       </c>
       <c r="M8" s="1">
         <f>E8-B8</f>
-        <v>420</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -854,17 +854,17 @@
         <v>1350</v>
       </c>
       <c r="E9" s="1">
-        <v>1800</v>
+        <v>1770</v>
       </c>
       <c r="F9" s="1">
-        <v>1000</v>
+        <v>980</v>
       </c>
       <c r="G9" s="1">
-        <v>850</v>
+        <v>900</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
@@ -872,19 +872,19 @@
       </c>
       <c r="J9" s="1">
         <f>E9</f>
-        <v>1800</v>
+        <v>1770</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>-450</v>
+        <v>-470</v>
       </c>
       <c r="M9" s="1">
         <f>B9-E9</f>
-        <v>-500</v>
+        <v>-470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DNM Fixing Sesi 1!
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAB57F4-BB50-48AC-B885-175EC96BACC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105AECF1-313F-4C1F-8188-3E461718F91E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5295" yWindow="720" windowWidth="15195" windowHeight="7875" tabRatio="442" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +707,7 @@
         <v>1400</v>
       </c>
       <c r="C6" s="1">
-        <v>1280</v>
+        <v>1180</v>
       </c>
       <c r="D6" s="1">
         <v>1680</v>
@@ -716,18 +716,18 @@
         <v>850</v>
       </c>
       <c r="F6" s="1">
-        <v>1800</v>
+        <v>1700</v>
       </c>
       <c r="G6" s="1">
-        <v>2180</v>
+        <v>2150</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2680</v>
+        <v>2620</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>1280</v>
+        <v>1180</v>
       </c>
       <c r="J6" s="1">
         <f>E6</f>
@@ -735,7 +735,7 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-500</v>
+        <v>-470</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Fixing Legs For 1,2, and 3
</commit_message>
<xml_diff>
--- a/krpai2020/Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Sesi 1/automatic calibration calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105AECF1-313F-4C1F-8188-3E461718F91E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C10E42-C6AF-48EB-8700-4A208CD2E658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5295" yWindow="720" windowWidth="15195" windowHeight="7875" tabRatio="442" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +851,7 @@
         <v>1450</v>
       </c>
       <c r="D9" s="1">
-        <v>1350</v>
+        <v>1300</v>
       </c>
       <c r="E9" s="1">
         <v>1770</v>
@@ -860,11 +860,11 @@
         <v>980</v>
       </c>
       <c r="G9" s="1">
-        <v>900</v>
+        <v>850</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>

</xml_diff>